<commit_message>
valueset and codesystem changes
</commit_message>
<xml_diff>
--- a/output/CodeSystem-nigeria-allergy-severity.xlsx
+++ b/output/CodeSystem-nigeria-allergy-severity.xlsx
@@ -36,13 +36,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>NigeriaAllergySeverityCS</t>
+    <t>NGAllergySeverityCS</t>
   </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>NG-Imm Reaction Severity CS</t>
+    <t>NG-Imm Allergy Severity CS</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-24T09:13:37+01:00</t>
+    <t>2025-06-25T06:29:04+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>